<commit_message>
new cramer rao bounds
</commit_message>
<xml_diff>
--- a/evaluation/mean_bounds.xlsx
+++ b/evaluation/mean_bounds.xlsx
@@ -491,12 +491,12 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Phi_phi0</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Phi_theta0</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Phi_phi0</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -512,46 +512,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0003465321643466667</v>
+        <v>0.0005865707428022582</v>
       </c>
       <c r="C2" t="n">
-        <v>7.58155532541048e-06</v>
+        <v>3.101067652844651e-08</v>
       </c>
       <c r="D2" t="n">
-        <v>9.045114042064114e-09</v>
+        <v>4.76923237286854e-10</v>
       </c>
       <c r="E2" t="n">
-        <v>2.172010149111357e-07</v>
+        <v>1.217627311888573e-09</v>
       </c>
       <c r="F2" t="n">
-        <v>-3.31256860287022e-07</v>
+        <v>-2.149355397241235e-09</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.448313384073119e-07</v>
+        <v>-2.943145147442055e-09</v>
       </c>
       <c r="H2" t="n">
-        <v>-4.361189879443255e-07</v>
+        <v>-2.207081446607662e-05</v>
       </c>
       <c r="I2" t="n">
-        <v>-5.749065333979637e-06</v>
+        <v>-1.364189471955363e-05</v>
       </c>
       <c r="J2" t="n">
-        <v>-8.780411944601009e-06</v>
+        <v>2.23736857949539e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>2.129281869280844e-06</v>
+        <v>-9.938916579172829e-06</v>
       </c>
       <c r="L2" t="n">
-        <v>-7.938360700764917e-06</v>
+        <v>6.683802486366034e-06</v>
       </c>
       <c r="M2" t="n">
-        <v>-6.776263358441153e-05</v>
+        <v>8.610866161386833e-05</v>
       </c>
       <c r="N2" t="n">
-        <v>-6.607257365365394e-05</v>
+        <v>0.0001217067026377315</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.0001775254872474468</v>
+        <v>0.0002358803922126165</v>
       </c>
     </row>
     <row r="3">
@@ -562,43 +562,43 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>1.752592383263635e-05</v>
+        <v>6.12233567191681e-11</v>
       </c>
       <c r="D3" t="n">
-        <v>2.170742024800426e-08</v>
+        <v>1.623206650674353e-11</v>
       </c>
       <c r="E3" t="n">
-        <v>4.870125572465835e-07</v>
+        <v>-6.363829484292395e-12</v>
       </c>
       <c r="F3" t="n">
-        <v>-7.180929406532833e-07</v>
+        <v>4.270705028095265e-12</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.813324750210768e-07</v>
+        <v>2.809788026041792e-12</v>
       </c>
       <c r="H3" t="n">
-        <v>5.638690435710314e-08</v>
+        <v>-1.932949147894004e-08</v>
       </c>
       <c r="I3" t="n">
-        <v>1.765580421381882e-06</v>
+        <v>3.298677412050234e-09</v>
       </c>
       <c r="J3" t="n">
-        <v>1.008199013275945e-06</v>
+        <v>-1.322792342254664e-09</v>
       </c>
       <c r="K3" t="n">
-        <v>-1.556940711945616e-06</v>
+        <v>-6.985411301524843e-09</v>
       </c>
       <c r="L3" t="n">
-        <v>1.131075686166618e-06</v>
+        <v>3.283835066933199e-09</v>
       </c>
       <c r="M3" t="n">
-        <v>-8.496207581113777e-05</v>
+        <v>-9.630816343488513e-08</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.0001014957660296571</v>
+        <v>3.50994249248629e-08</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.0005039262574843766</v>
+        <v>-1.450560043107301e-07</v>
       </c>
     </row>
     <row r="4">
@@ -610,40 +610,40 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>9.327040391012074e-10</v>
+        <v>4.846513084217753e-11</v>
       </c>
       <c r="E4" t="n">
-        <v>6.571167318637545e-10</v>
+        <v>-3.060066258302464e-13</v>
       </c>
       <c r="F4" t="n">
-        <v>-8.518458631220918e-10</v>
+        <v>2.192492027873383e-13</v>
       </c>
       <c r="G4" t="n">
-        <v>-6.031544634582018e-09</v>
+        <v>-3.902789762772377e-11</v>
       </c>
       <c r="H4" t="n">
-        <v>2.108439357765789e-09</v>
+        <v>2.996140051948911e-09</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.919321757765837e-09</v>
+        <v>3.633962267949914e-09</v>
       </c>
       <c r="J4" t="n">
-        <v>2.127335582491754e-08</v>
+        <v>-9.374353840181265e-10</v>
       </c>
       <c r="K4" t="n">
-        <v>3.746658498945795e-09</v>
+        <v>1.078494016713809e-08</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.946871312709781e-08</v>
+        <v>1.708181586882974e-08</v>
       </c>
       <c r="M4" t="n">
-        <v>4.44323728070932e-06</v>
+        <v>-2.653782791289729e-07</v>
       </c>
       <c r="N4" t="n">
-        <v>-3.149393041734623e-06</v>
+        <v>2.285532895614608e-07</v>
       </c>
       <c r="O4" t="n">
-        <v>-1.686934792934252e-07</v>
+        <v>-4.787361765700931e-08</v>
       </c>
     </row>
     <row r="5">
@@ -656,37 +656,37 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>1.427366661615156e-08</v>
+        <v>3.362010712423705e-12</v>
       </c>
       <c r="F5" t="n">
-        <v>-2.050637791338348e-08</v>
+        <v>-2.380107134266269e-12</v>
       </c>
       <c r="G5" t="n">
-        <v>-6.901512134036798e-09</v>
+        <v>-3.124884629242691e-12</v>
       </c>
       <c r="H5" t="n">
-        <v>1.999239401230071e-09</v>
+        <v>-6.265488494255017e-09</v>
       </c>
       <c r="I5" t="n">
-        <v>4.891831939731438e-08</v>
+        <v>-3.210061486853674e-10</v>
       </c>
       <c r="J5" t="n">
-        <v>1.809981337779442e-08</v>
+        <v>4.355921438090672e-10</v>
       </c>
       <c r="K5" t="n">
-        <v>-4.981130933536753e-08</v>
+        <v>7.776594098431285e-10</v>
       </c>
       <c r="L5" t="n">
-        <v>2.016760845111653e-08</v>
+        <v>-3.077394067943565e-09</v>
       </c>
       <c r="M5" t="n">
-        <v>-1.913658853522867e-06</v>
+        <v>-2.714223289424777e-08</v>
       </c>
       <c r="N5" t="n">
-        <v>-3.694627310977713e-06</v>
+        <v>-2.11591505308449e-08</v>
       </c>
       <c r="O5" t="n">
-        <v>-5.739183133549423e-06</v>
+        <v>2.846239149653389e-08</v>
       </c>
     </row>
     <row r="6">
@@ -700,34 +700,34 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>3.043745981803631e-08</v>
+        <v>2.614607825925151e-12</v>
       </c>
       <c r="G6" t="n">
-        <v>6.97104683099418e-09</v>
+        <v>1.623029747288337e-12</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.179828391724978e-09</v>
+        <v>2.807436162137531e-08</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.517423032769108e-08</v>
+        <v>-2.878306849915708e-10</v>
       </c>
       <c r="J6" t="n">
-        <v>-2.483216246339493e-08</v>
+        <v>-9.690951294949218e-10</v>
       </c>
       <c r="K6" t="n">
-        <v>8.470131452808927e-08</v>
+        <v>2.56476600227827e-10</v>
       </c>
       <c r="L6" t="n">
-        <v>1.519511538201084e-08</v>
+        <v>-8.91299310853885e-10</v>
       </c>
       <c r="M6" t="n">
-        <v>4.684010782021103e-06</v>
+        <v>4.73089343297891e-08</v>
       </c>
       <c r="N6" t="n">
-        <v>5.068299653723471e-06</v>
+        <v>4.191687930943955e-08</v>
       </c>
       <c r="O6" t="n">
-        <v>1.394920939230699e-05</v>
+        <v>2.276717957602607e-09</v>
       </c>
     </row>
     <row r="7">
@@ -742,31 +742,31 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>1.198461800851094e-06</v>
+        <v>4.166290235743476e-11</v>
       </c>
       <c r="H7" t="n">
-        <v>-4.346667930650122e-07</v>
+        <v>1.453144874452881e-09</v>
       </c>
       <c r="I7" t="n">
-        <v>-3.099674157265396e-07</v>
+        <v>-2.258239862054472e-09</v>
       </c>
       <c r="J7" t="n">
-        <v>4.571813777730041e-07</v>
+        <v>4.423353537295178e-10</v>
       </c>
       <c r="K7" t="n">
-        <v>-3.68976851533913e-06</v>
+        <v>-1.841641977164669e-08</v>
       </c>
       <c r="L7" t="n">
-        <v>4.063877584788018e-06</v>
+        <v>-3.354091178562904e-08</v>
       </c>
       <c r="M7" t="n">
-        <v>-5.635850024663594e-05</v>
+        <v>2.94562800927592e-07</v>
       </c>
       <c r="N7" t="n">
-        <v>-3.050171327684558e-06</v>
+        <v>-1.081899147480721e-07</v>
       </c>
       <c r="O7" t="n">
-        <v>-2.551778793075189e-05</v>
+        <v>-8.413375929841176e-08</v>
       </c>
     </row>
     <row r="8">
@@ -782,28 +782,28 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>0.001775061566974485</v>
+        <v>0.002422240117188004</v>
       </c>
       <c r="I8" t="n">
-        <v>-8.305774962202674e-05</v>
+        <v>-2.2147135736164e-05</v>
       </c>
       <c r="J8" t="n">
-        <v>-3.755071522492984e-05</v>
+        <v>-1.783004619602197e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0005527474480954217</v>
+        <v>9.729648590519111e-05</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0003152212403586134</v>
+        <v>0.0001440123414253604</v>
       </c>
       <c r="M8" t="n">
-        <v>2.036072600232043e-06</v>
+        <v>0.001487490293657892</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.0003143226070783986</v>
+        <v>0.00125524280802329</v>
       </c>
       <c r="O8" t="n">
-        <v>1.409806871257126e-05</v>
+        <v>-0.0003142943039060382</v>
       </c>
     </row>
     <row r="9">
@@ -820,25 +820,25 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>0.001504959522800361</v>
+        <v>0.002232303694120674</v>
       </c>
       <c r="J9" t="n">
-        <v>6.77098442219368e-05</v>
+        <v>2.165489783586008e-05</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0004983111161459485</v>
+        <v>-0.001030141029337531</v>
       </c>
       <c r="L9" t="n">
-        <v>0.001203163142163906</v>
+        <v>0.0008220734456962875</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0002362692530651878</v>
+        <v>4.293781999946261e-06</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.841493358228427e-05</v>
+        <v>0.0001879391457534538</v>
       </c>
       <c r="O9" t="n">
-        <v>-8.459126664888254e-05</v>
+        <v>0.0001178874965792063</v>
       </c>
     </row>
     <row r="10">
@@ -856,22 +856,22 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
-        <v>0.002941498042013507</v>
+        <v>0.0003533587771233257</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0001831376252500194</v>
+        <v>-1.615476956471619e-05</v>
       </c>
       <c r="L10" t="n">
-        <v>6.001801886477681e-05</v>
+        <v>0.0002760442350934531</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0002110985812728046</v>
+        <v>-8.99426471558907e-05</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0004889769838289701</v>
+        <v>-9.827263126949856e-06</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.0001775927550392354</v>
+        <v>-5.86232975499785e-06</v>
       </c>
     </row>
     <row r="11">
@@ -890,19 +890,19 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>0.005617128381025517</v>
+        <v>0.02656093706752399</v>
       </c>
       <c r="L11" t="n">
-        <v>0.001634628568085086</v>
+        <v>0.01207856161886289</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.001434429414394375</v>
+        <v>-0.0129523303797163</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.001147563217126087</v>
+        <v>0.1173198877868248</v>
       </c>
       <c r="O11" t="n">
-        <v>1.523111399211834e-05</v>
+        <v>-0.0001247682940825344</v>
       </c>
     </row>
     <row r="12">
@@ -922,22 +922,22 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
-        <v>0.06570437043966772</v>
+        <v>0.1690812681821677</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0001846044323974061</v>
+        <v>-0.1200937770874017</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.06157032944053899</v>
+        <v>0.1024552451204341</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0001528219688264447</v>
+        <v>0.0004649557183792104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Phi_theta0</t>
+          <t>Phi_phi0</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -952,19 +952,19 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>0.1418585567700322</v>
+        <v>0.1986720829524958</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0454572209672171</v>
+        <v>-0.06162235256176028</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.003091469350534887</v>
+        <v>-0.005354331767963187</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Phi_phi0</t>
+          <t>Phi_theta0</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -980,10 +980,10 @@
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
-        <v>0.1579036020681195</v>
+        <v>1.056799840188618</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.01043975873518005</v>
+        <v>-0.005290252050545846</v>
       </c>
     </row>
     <row r="15">
@@ -1006,7 +1006,7 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="n">
-        <v>0.2808155629094506</v>
+        <v>0.0479951001769764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>